<commit_message>
Restructuring, better layout of evaluation and appendix
</commit_message>
<xml_diff>
--- a/data/TesslaServer Number of Events Benchmark.xlsx
+++ b/data/TesslaServer Number of Events Benchmark.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
   <si>
     <t>V1</t>
   </si>
@@ -115,7 +115,19 @@
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
     <cellStyle name="Überschrift 1" xfId="1" builtinId="16"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="23">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#0.###0\ &quot;s&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#0.###0\ &quot;s&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#0.###0\ &quot;s&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#0.###0\ &quot;s&quot;"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="#0.###0\ &quot;s&quot;"/>
     </dxf>
@@ -168,15 +180,6 @@
           <color theme="4"/>
         </top>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#0.###0\ &quot;s&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#0.###0\ &quot;s&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#0.###0\ &quot;s&quot;"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="#0.###0\ &quot;s&quot;"/>
@@ -242,6 +245,34 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>Timeout</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:numFmt formatCode="#0.###0\ &quot;s&quot;" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -321,10 +352,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$24:$D$24</c:f>
+              <c:f>Tabelle1!$B$24:$E$24</c:f>
               <c:numCache>
-                <c:formatCode>#0.###0\ "s"</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:formatCode>#0#,##0\ "s"</c:formatCode>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0.58424402475357</c:v>
                 </c:pt>
@@ -333,6 +364,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>24.84564189910889</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -465,11 +499,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-771109664"/>
-        <c:axId val="-752730560"/>
+        <c:axId val="-1184261856"/>
+        <c:axId val="-1182432720"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-771109664"/>
+        <c:axId val="-1184261856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -568,7 +602,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-752730560"/>
+        <c:crossAx val="-1182432720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -576,9 +610,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-752730560"/>
+        <c:axId val="-1182432720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="30.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -683,7 +718,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-771109664"/>
+        <c:crossAx val="-1184261856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1313,8 +1348,8 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
@@ -1343,38 +1378,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Version1" displayName="Version1" ref="B3:D24" totalsRowCount="1" tableBorderDxfId="21">
-  <autoFilter ref="B3:D23"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="500" totalsRowFunction="average" dataDxfId="20" totalsRowDxfId="19"/>
-    <tableColumn id="2" name="1000" totalsRowFunction="average" dataDxfId="18" totalsRowDxfId="17"/>
-    <tableColumn id="3" name="5000" totalsRowFunction="average" dataDxfId="16" totalsRowDxfId="15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Version1" displayName="Version1" ref="B3:E24" totalsRowCount="1" tableBorderDxfId="22">
+  <autoFilter ref="B3:E23"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="500" totalsRowFunction="average" dataDxfId="21" totalsRowDxfId="2"/>
+    <tableColumn id="2" name="1000" totalsRowFunction="average" dataDxfId="20" totalsRowDxfId="1"/>
+    <tableColumn id="3" name="5000" totalsRowFunction="average" dataDxfId="19" totalsRowDxfId="0"/>
+    <tableColumn id="4" name="10000" totalsRowFunction="average" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Version1.5" displayName="Version1.5" ref="B27:E48" totalsRowCount="1" tableBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Version1.5" displayName="Version1.5" ref="B27:E48" totalsRowCount="1" tableBorderDxfId="18">
   <autoFilter ref="B27:E47"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="500" totalsRowFunction="average" dataDxfId="13"/>
-    <tableColumn id="2" name="1000" totalsRowFunction="average" dataDxfId="12"/>
-    <tableColumn id="3" name="5000" totalsRowFunction="average" dataDxfId="11"/>
-    <tableColumn id="4" name="10000" totalsRowFunction="average" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="1" name="500" totalsRowFunction="average" dataDxfId="17"/>
+    <tableColumn id="2" name="1000" totalsRowFunction="average" dataDxfId="16"/>
+    <tableColumn id="3" name="5000" totalsRowFunction="average" dataDxfId="15"/>
+    <tableColumn id="4" name="10000" totalsRowFunction="average" dataDxfId="14" totalsRowDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Version2" displayName="Version2" ref="B51:E72" totalsRowCount="1" tableBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Version2" displayName="Version2" ref="B51:E72" totalsRowCount="1" tableBorderDxfId="12">
   <autoFilter ref="B51:E71"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="500" totalsRowFunction="average" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="2" name="1000" totalsRowFunction="average" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="3" name="5000" totalsRowFunction="average" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="4" name="10000" totalsRowFunction="average" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="1" name="500" totalsRowFunction="average" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="2" name="1000" totalsRowFunction="average" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="3" name="5000" totalsRowFunction="average" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="4" name="10000" totalsRowFunction="average" dataDxfId="5" totalsRowDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1646,7 +1682,7 @@
   <dimension ref="B2:E72"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:E47"/>
+      <selection activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1654,14 +1690,14 @@
     <col min="2" max="5" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="20" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" ht="20" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -1671,8 +1707,11 @@
       <c r="D3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="1">
         <v>0.58151412010192904</v>
       </c>
@@ -1682,8 +1721,11 @@
       <c r="D4" s="1">
         <v>39.004570007324197</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E4" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
         <v>0.59580397605895996</v>
       </c>
@@ -1693,8 +1735,9 @@
       <c r="D5" s="1">
         <v>33.577141046523998</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="1">
         <v>0.596333026885986</v>
       </c>
@@ -1704,8 +1747,9 @@
       <c r="D6" s="1">
         <v>26.825165987014799</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" s="1">
         <v>0.57996106147766102</v>
       </c>
@@ -1715,8 +1759,9 @@
       <c r="D7" s="1">
         <v>23.894372940063501</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" s="1">
         <v>0.59483003616332997</v>
       </c>
@@ -1726,8 +1771,9 @@
       <c r="D8" s="1">
         <v>23.8836619853973</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B9" s="1">
         <v>0.58247590065002397</v>
       </c>
@@ -1737,8 +1783,9 @@
       <c r="D9" s="1">
         <v>23.410987138748201</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B10" s="1">
         <v>0.62713003158569303</v>
       </c>
@@ -1748,8 +1795,9 @@
       <c r="D10" s="1">
         <v>23.192898988723801</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B11" s="1">
         <v>0.57050991058349598</v>
       </c>
@@ -1759,8 +1807,9 @@
       <c r="D11" s="1">
         <v>23.322654962539701</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B12" s="1">
         <v>0.57645106315612804</v>
       </c>
@@ -1770,8 +1819,9 @@
       <c r="D12" s="1">
         <v>21.904250860214201</v>
       </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B13" s="1">
         <v>0.58930897712707497</v>
       </c>
@@ -1781,8 +1831,9 @@
       <c r="D13" s="1">
         <v>22.951647996902501</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B14" s="1">
         <v>0.61006999015808105</v>
       </c>
@@ -1792,8 +1843,9 @@
       <c r="D14" s="1">
         <v>22.837744951248201</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B15" s="1">
         <v>0.56840205192565896</v>
       </c>
@@ -1803,8 +1855,9 @@
       <c r="D15" s="1">
         <v>26.197367906570399</v>
       </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B16" s="1">
         <v>0.57460403442382801</v>
       </c>
@@ -1814,6 +1867,7 @@
       <c r="D16" s="1">
         <v>25.753642082214402</v>
       </c>
+      <c r="E16" s="1"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" s="1">
@@ -1825,6 +1879,7 @@
       <c r="D17" s="1">
         <v>24.6288599967957</v>
       </c>
+      <c r="E17" s="1"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" s="1">
@@ -1836,6 +1891,7 @@
       <c r="D18" s="1">
         <v>22.370877981185899</v>
       </c>
+      <c r="E18" s="1"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" s="1">
@@ -1847,6 +1903,7 @@
       <c r="D19" s="1">
         <v>23.940432071685802</v>
       </c>
+      <c r="E19" s="1"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" s="1">
@@ -1858,6 +1915,7 @@
       <c r="D20" s="1">
         <v>21.4452769756317</v>
       </c>
+      <c r="E20" s="1"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" s="1">
@@ -1869,6 +1927,7 @@
       <c r="D21" s="1">
         <v>23.348201036453201</v>
       </c>
+      <c r="E21" s="1"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" s="1">
@@ -1880,6 +1939,7 @@
       <c r="D22" s="1">
         <v>21.975319862365701</v>
       </c>
+      <c r="E22" s="1"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" s="1">
@@ -1891,6 +1951,7 @@
       <c r="D23" s="1">
         <v>22.447763204574599</v>
       </c>
+      <c r="E23" s="1"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" s="1">
@@ -1904,6 +1965,10 @@
       <c r="D24" s="1">
         <f>SUBTOTAL(101,Version1[5000])</f>
         <v>24.845641899108891</v>
+      </c>
+      <c r="E24" s="1">
+        <f>SUBTOTAL(101,Version1[10000])</f>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="2:5" ht="20" x14ac:dyDescent="0.25">

</xml_diff>